<commit_message>
added midt seminar to gantt
</commit_message>
<xml_diff>
--- a/res/tidsplan p1.xlsx
+++ b/res/tidsplan p1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programs\P1\AAU_p1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programs\P1\AAU_p1\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573B4A45-1759-4057-8897-A58BAE730349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6929B4-99D6-49FC-8288-A5352FA21C41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Fremhæv et tidsrum til højre.  Derpå følger en forklaring af diagrammet.</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>UML class diagram</t>
+  </si>
+  <si>
+    <t>Midtvejs seminar</t>
   </si>
 </sst>
 </file>
@@ -567,6 +570,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="18" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="8" borderId="1" xfId="13" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -617,15 +629,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="8" borderId="1" xfId="13" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1038,8 +1041,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="49" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="49" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1097,13 +1100,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1111,69 +1114,69 @@
         <v>50</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="30"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="20" t="s">
+      <c r="V2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="33"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="34" t="s">
+      <c r="AA2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="39"/>
       <c r="AH2" s="19"/>
-      <c r="AI2" s="20" t="s">
+      <c r="AI2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
+      <c r="AJ2" s="24"/>
+      <c r="AK2" s="24"/>
+      <c r="AL2" s="24"/>
+      <c r="AM2" s="24"/>
+      <c r="AN2" s="24"/>
+      <c r="AO2" s="24"/>
+      <c r="AP2" s="24"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="38" t="str">
+      <c r="H3" s="21" t="str">
         <f>"12/10"</f>
         <v>12/10</v>
       </c>
@@ -1229,20 +1232,20 @@
         <f>"14/12"</f>
         <v>14/12</v>
       </c>
-      <c r="BD3" s="37"/>
+      <c r="BD3" s="20"/>
       <c r="BE3" s="10" t="str">
         <f>"18/12"</f>
         <v>18/12</v>
       </c>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="38">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="21">
         <v>1</v>
       </c>
       <c r="I4" s="3">
@@ -1424,7 +1427,7 @@
       </c>
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="22" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7">
@@ -1444,7 +1447,7 @@
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="7">
@@ -1464,7 +1467,7 @@
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="7">
@@ -1484,7 +1487,7 @@
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="7">
@@ -1498,7 +1501,7 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7">
@@ -1512,7 +1515,7 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="7">
@@ -1526,7 +1529,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="7">
@@ -1540,7 +1543,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="7">
@@ -1554,15 +1557,25 @@
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="39"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="7">
+        <v>27</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
+        <v>27</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="39"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1570,7 +1583,7 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="39"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1578,7 +1591,7 @@
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="39"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1602,7 +1615,7 @@
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="7">
@@ -1616,7 +1629,7 @@
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="22" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="7">
@@ -1630,7 +1643,7 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="7">
@@ -1644,7 +1657,7 @@
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="7">
@@ -1714,7 +1727,7 @@
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="39"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>

</xml_diff>